<commit_message>
[API FINISHED] refactor upload file
</commit_message>
<xml_diff>
--- a/api-reactjs-project/uploads/score/005.xlsx
+++ b/api-reactjs-project/uploads/score/005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ggj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E305DC-0B5F-9A4D-B471-DEA40208A182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AE9610-9F32-F546-8828-1BAE3E620324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7300" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{19EED111-B38F-5641-8AAB-D31D7E327387}"/>
   </bookViews>
@@ -408,7 +408,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,7 +443,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>